<commit_message>
feat: Add new Excel sample files and refactor data export functions to support multiple sheets and metadata handling
</commit_message>
<xml_diff>
--- a/data/sample_padrao1.xlsx
+++ b/data/sample_padrao1.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="11_2B5A8FE7125C5C426140C57430267256DF8CDB53" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4E2B62C-9212-4CEC-BDBA-995878A0D215}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="11_2B5A8FE7125C5C426140C57430267256DF8CDB53" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE36E1D7-9C86-4666-8A76-CB86835F6450}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Resumo" sheetId="1" r:id="rId1"/>
-    <sheet name="01" sheetId="2" r:id="rId2"/>
+    <sheet name="Resumo" sheetId="2" r:id="rId1"/>
+    <sheet name="01" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -627,10 +627,151 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>10.5</v>
+      </c>
+      <c r="E5">
+        <v>119.37</v>
+      </c>
+      <c r="F5">
+        <v>1.3</v>
+      </c>
+      <c r="G5">
+        <v>1629.4005</v>
+      </c>
+      <c r="H5">
+        <v>30.02138456431106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>369.84</v>
+      </c>
+      <c r="F6">
+        <v>1.3</v>
+      </c>
+      <c r="G6">
+        <v>2403.96</v>
+      </c>
+      <c r="H6">
+        <v>44.292491402341668</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>26.85</v>
+      </c>
+      <c r="E7">
+        <v>39.94</v>
+      </c>
+      <c r="F7">
+        <v>1.3</v>
+      </c>
+      <c r="G7">
+        <v>1394.1057000000001</v>
+      </c>
+      <c r="H7">
+        <v>25.686124033347269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8">
+        <v>5427.4661999999998</v>
+      </c>
+      <c r="H8">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -3402,145 +3543,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>10.5</v>
-      </c>
-      <c r="E5">
-        <v>119.37</v>
-      </c>
-      <c r="F5">
-        <v>1.3</v>
-      </c>
-      <c r="G5">
-        <v>1629.4005</v>
-      </c>
-      <c r="H5">
-        <v>30.02138456431106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>369.84</v>
-      </c>
-      <c r="F6">
-        <v>1.3</v>
-      </c>
-      <c r="G6">
-        <v>2403.96</v>
-      </c>
-      <c r="H6">
-        <v>44.292491402341668</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>26.85</v>
-      </c>
-      <c r="E7">
-        <v>39.94</v>
-      </c>
-      <c r="F7">
-        <v>1.3</v>
-      </c>
-      <c r="G7">
-        <v>1394.1057000000001</v>
-      </c>
-      <c r="H7">
-        <v>25.686124033347269</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8">
-        <v>5427.4661999999998</v>
-      </c>
-      <c r="H8">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>